<commit_message>
Add Scene switch and ending
</commit_message>
<xml_diff>
--- a/ExcelData/Ending.xlsx
+++ b/ExcelData/Ending.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7A56FCD-F62B-4EFA-93E7-CC195ADCB666}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51504B0F-632A-4F7B-9FF2-A814864D8FA7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>结局编号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -38,23 +38,43 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>结局1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>结局2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>结局3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>结局4</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>结局5</t>
+    <t>健身是一种信仰，你成为了一名健美教练。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>你活蹦乱跳，体能过人，在小学时体育老师发现了你的天赋，你立志成为一名运动员~</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>你对这五彩缤纷的世界有独特的美的感受，画画让你沉醉，成为一名艺术生快乐地画画是你的理想~</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>你成为了一名国家级运动员，在赛场上挥洒汗水让你十分激动自豪。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>孩子们健康茁壮的成长让你欣慰，体育老师就是你热爱的职业。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>体育也是一门科学，你考入大学进行体育理论相关的学习与深造。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>艺术来自生活，你汲取生活中的美画成了多本漫画，作为一名漫画家你感到十分快乐。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>你的画作在比赛上获奖，获得了众多赞美，被认可感与成就感让你更加热爱画画。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>你的职业并不是画画相关，但画画让你的生活更加快乐，是你带给你诸多快乐的爱好。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>你成为了一名美术老师，学生们可爱的画作让你感到自己工作的充实与幸福。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -380,10 +400,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -418,7 +438,7 @@
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -426,13 +446,13 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -446,7 +466,7 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -454,10 +474,10 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D5" t="s">
         <v>7</v>
@@ -468,13 +488,83 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D6" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="D10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="D11" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>